<commit_message>
Move CCS duration adjustment into input data.
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\CS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DA79CC-9A9E-497B-AC5C-A53C6DD175A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A59A9D-1519-4868-94FE-D55646C4FFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="BCS" sheetId="4" r:id="rId2"/>
+    <sheet name="Electricity Calculations" sheetId="5" r:id="rId2"/>
+    <sheet name="BCS" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">About!$A$10</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">About!$A$11</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -31,7 +32,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">About!$A$8</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">About!$A$9</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Source:</t>
   </si>
@@ -90,6 +91,21 @@
   </si>
   <si>
     <t>45Q Tax Credit Amount</t>
+  </si>
+  <si>
+    <t>Credit Amount</t>
+  </si>
+  <si>
+    <t>Repayment Period for Financing</t>
+  </si>
+  <si>
+    <t>45Q Credit Duration</t>
+  </si>
+  <si>
+    <t>Credit Value</t>
+  </si>
+  <si>
+    <t>For electricity, adjust the credit value based on its duration relative to the financing repayment period</t>
   </si>
 </sst>
 </file>
@@ -145,7 +161,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -155,7 +171,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -176,9 +193,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -216,9 +233,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,26 +268,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,26 +303,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -496,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,19 +515,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>0.78500000000000003</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B11" s="6">
         <v>85</v>
       </c>
     </row>
@@ -555,6 +543,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB35C55-7F27-44A6-A8A7-496D78F28576}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7">
+        <f>About!B11</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
+        <f>B1*B3/B2</f>
+        <v>42.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -562,7 +602,7 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="D2" sqref="D2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,44 +717,44 @@
         <v>0</v>
       </c>
       <c r="D2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="E2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="F2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="G2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="H2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="I2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="J2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="K2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="L2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="M2" s="7">
-        <f>About!$B$10*About!$A$8</f>
-        <v>66.725000000000009</v>
+        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
+        <v>33.362500000000004</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -781,44 +821,44 @@
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="D3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="E3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="E3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="F3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="F3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="G3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="G3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="H3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="H3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="I3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="I3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="J3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="J3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="K3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="K3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="L3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="L3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
-      <c r="M3" s="7">
-        <f>About!$B$10*About!$A$8</f>
+      <c r="M3">
+        <f>About!$B$11*About!$A$9</f>
         <v>66.725000000000009</v>
       </c>
       <c r="N3">

</xml_diff>

<commit_message>
Updates correcting CCS subsidy duration to 12 years in IRA (previously was erroneously entered as 10 years).
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A59A9D-1519-4868-94FE-D55646C4FFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EB2AB3-FE1A-4C06-98D6-C7F0874829B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29670" yWindow="2655" windowWidth="26940" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,7 +172,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -482,7 +481,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +515,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -547,7 +546,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +576,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -586,7 +585,7 @@
       </c>
       <c r="B4" s="7">
         <f>B1*B3/B2</f>
-        <v>42.5</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -718,43 +717,43 @@
       </c>
       <c r="D2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="E2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="F2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="G2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="H2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="I2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="J2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="K2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="L2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="M2" s="7">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>33.362500000000004</v>
+        <v>40.035000000000004</v>
       </c>
       <c r="N2">
         <v>0</v>

</xml_diff>

<commit_message>
Fixes to format for CCS subsidies.
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\Kentucky\eps-kentucky\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EB2AB3-FE1A-4C06-98D6-C7F0874829B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4980F67B-0D0E-4942-ABFD-8FB5DFE0CDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29670" yWindow="2655" windowWidth="26940" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,6 +172,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -480,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -600,7 +601,7 @@
   </sheetPr>
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:M2"/>
     </sheetView>
   </sheetViews>
@@ -715,43 +716,43 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="8">
         <f>'Electricity Calculations'!$B$4*About!$A$9</f>
         <v>40.035000000000004</v>
       </c>

</xml_diff>

<commit_message>
Updates data used for cost of capital in the electricity sector. Integrates tax credit deflators and timelines into the estimates for cost per unit new elec output and separately for dispatch costs. Recalibrates CSC parameters.
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\Kentucky\eps-kentucky\InputData\ccs\BCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4980F67B-0D0E-4942-ABFD-8FB5DFE0CDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F268FE25-6FA1-4964-97BE-7705BD55074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Electricity Calculations" sheetId="5" r:id="rId2"/>
-    <sheet name="BCS" sheetId="4" r:id="rId3"/>
+    <sheet name="BCS-BCS" sheetId="4" r:id="rId3"/>
+    <sheet name="BCS-DoSfCS" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">About!$A$11</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Source:</t>
   </si>
@@ -106,6 +107,18 @@
   </si>
   <si>
     <t>For electricity, adjust the credit value based on its duration relative to the financing repayment period</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>45Q Duration</t>
+  </si>
+  <si>
+    <t>12 years</t>
   </si>
 </sst>
 </file>
@@ -161,7 +174,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -172,7 +185,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -479,25 +491,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="55.88671875" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,22 +517,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>0.78500000000000003</v>
       </c>
@@ -528,12 +540,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="6">
         <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -550,12 +570,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -564,7 +584,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -572,7 +592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -580,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -601,17 +621,17 @@
   </sheetPr>
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -706,7 +726,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -716,45 +736,45 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="E2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="F2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="G2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="H2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="I2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="J2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="K2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="L2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
-      </c>
-      <c r="M2" s="8">
-        <f>'Electricity Calculations'!$B$4*About!$A$9</f>
-        <v>40.035000000000004</v>
+      <c r="D2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="E2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="F2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="G2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="H2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="I2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="J2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="K2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="L2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
+      </c>
+      <c r="M2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>66.725000000000009</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -811,7 +831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -914,6 +934,243 @@
       </c>
       <c r="AE3">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5698252-CD29-4D86-9D7F-2214C5598602}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>2021</v>
+      </c>
+      <c r="C1">
+        <v>2022</v>
+      </c>
+      <c r="D1">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2024</v>
+      </c>
+      <c r="F1">
+        <v>2025</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+      <c r="H1">
+        <v>2027</v>
+      </c>
+      <c r="I1">
+        <v>2028</v>
+      </c>
+      <c r="J1">
+        <v>2029</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1">
+        <v>2031</v>
+      </c>
+      <c r="M1">
+        <v>2032</v>
+      </c>
+      <c r="N1">
+        <v>2033</v>
+      </c>
+      <c r="O1">
+        <v>2034</v>
+      </c>
+      <c r="P1">
+        <v>2035</v>
+      </c>
+      <c r="Q1">
+        <v>2036</v>
+      </c>
+      <c r="R1">
+        <v>2037</v>
+      </c>
+      <c r="S1">
+        <v>2038</v>
+      </c>
+      <c r="T1">
+        <v>2039</v>
+      </c>
+      <c r="U1">
+        <v>2040</v>
+      </c>
+      <c r="V1">
+        <v>2041</v>
+      </c>
+      <c r="W1">
+        <v>2042</v>
+      </c>
+      <c r="X1">
+        <v>2043</v>
+      </c>
+      <c r="Y1">
+        <v>2044</v>
+      </c>
+      <c r="Z1">
+        <v>2045</v>
+      </c>
+      <c r="AA1">
+        <v>2046</v>
+      </c>
+      <c r="AB1">
+        <v>2047</v>
+      </c>
+      <c r="AC1">
+        <v>2048</v>
+      </c>
+      <c r="AD1">
+        <v>2049</v>
+      </c>
+      <c r="AE1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <f>$B$2</f>
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <f>$B$2</f>
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:AE2" si="0">$B$2</f>
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="R2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="U2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="V2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="W2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="X2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AA2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AB2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AC2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="AE2">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove IRA and EPA regs from recently edited files
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F268FE25-6FA1-4964-97BE-7705BD55074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEE04AC-F20D-4961-BFF8-FD6C6D2A3949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -497,19 +497,19 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="55.88671875" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,22 +517,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>0.78500000000000003</v>
       </c>
@@ -540,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -548,7 +548,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -570,12 +570,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -584,7 +584,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -592,7 +592,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -600,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -622,16 +622,16 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M2"/>
+      <selection activeCell="C2" sqref="C2:M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -726,7 +726,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -736,45 +736,35 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="E2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="F2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="G2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="H2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="I2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="J2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="K2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="L2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="M2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -831,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -841,45 +831,35 @@
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="E3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="F3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="G3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="H3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="I3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="J3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="K3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="L3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="M3">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -952,9 +932,9 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1049,7 +1029,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Edit currency year conversions for tax credits
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F268FE25-6FA1-4964-97BE-7705BD55074C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4713F7CF-0A9E-46D6-8386-EAB51C9BD0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Source:</t>
   </si>
@@ -79,9 +79,6 @@
     <t>None needed</t>
   </si>
   <si>
-    <t>2022 to 2012 USD</t>
-  </si>
-  <si>
     <t>This variable captures any BAU subsidies for CCS, specified in dollars per ton captured.</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>45Q Tax Credit Amount</t>
   </si>
   <si>
-    <t>Credit Amount</t>
-  </si>
-  <si>
     <t>Repayment Period for Financing</t>
   </si>
   <si>
@@ -119,6 +113,18 @@
   </si>
   <si>
     <t>12 years</t>
+  </si>
+  <si>
+    <t>https://www.bls.gov/data/inflation_calculator.htm</t>
+  </si>
+  <si>
+    <t>2024 to 2012 USD</t>
+  </si>
+  <si>
+    <t>Credit Amount, 2012 USD</t>
+  </si>
+  <si>
+    <t>*inflation adjusted starting in 2025, so we use the 2024 currency year to adjust to 2012 $</t>
   </si>
 </sst>
 </file>
@@ -174,7 +180,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -185,6 +191,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -491,25 +498,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="55.88671875" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,43 +524,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>0.78500000000000003</v>
+        <v>0.73</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="6">
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -570,43 +586,43 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B1" s="7">
-        <f>About!B11</f>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <f>About!B11*About!A9</f>
+        <v>62.05</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="7">
         <f>B1*B3/B2</f>
-        <v>51</v>
+        <v>37.229999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -622,18 +638,18 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:M2"/>
+      <selection activeCell="G2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2">
         <v>2021</v>
@@ -726,7 +742,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -736,45 +752,45 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="E2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="F2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="G2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="H2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="I2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="J2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="K2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="L2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
-      </c>
-      <c r="M2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+      <c r="D2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="E2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="F2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="G2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="H2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="I2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="J2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="K2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="L2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="M2" s="8">
+        <f>'Electricity Calculations'!$B$4</f>
+        <v>37.229999999999997</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -831,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -843,43 +859,43 @@
       </c>
       <c r="D3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="E3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="F3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="G3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="H3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="I3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="J3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="K3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="L3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="M3">
         <f>About!$B$11*About!$A$9</f>
-        <v>66.725000000000009</v>
+        <v>62.05</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -952,11 +968,11 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>2021</v>
@@ -1049,9 +1065,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>12</v>

</xml_diff>

<commit_message>
Fix to electricity sector BAU CCS subsidy values
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4713F7CF-0A9E-46D6-8386-EAB51C9BD0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB3F35D-7F66-4C00-89AD-AA6C0182CF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="Electricity Calculations" sheetId="5" r:id="rId2"/>
-    <sheet name="BCS-BCS" sheetId="4" r:id="rId3"/>
-    <sheet name="BCS-DoSfCS" sheetId="6" r:id="rId4"/>
+    <sheet name="BCS-BCS" sheetId="4" r:id="rId2"/>
+    <sheet name="BCS-DoSfCS" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">About!$A$11</definedName>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Source:</t>
   </si>
@@ -91,15 +90,6 @@
     <t>45Q Tax Credit Amount</t>
   </si>
   <si>
-    <t>Repayment Period for Financing</t>
-  </si>
-  <si>
-    <t>45Q Credit Duration</t>
-  </si>
-  <si>
-    <t>Credit Value</t>
-  </si>
-  <si>
     <t>For electricity, adjust the credit value based on its duration relative to the financing repayment period</t>
   </si>
   <si>
@@ -121,10 +111,13 @@
     <t>2024 to 2012 USD</t>
   </si>
   <si>
-    <t>Credit Amount, 2012 USD</t>
-  </si>
-  <si>
     <t>*inflation adjusted starting in 2025, so we use the 2024 currency year to adjust to 2012 $</t>
+  </si>
+  <si>
+    <t>45Q tax credits include a commenced construction provision. Based on EIA data, we assume a construction timeline</t>
+  </si>
+  <si>
+    <t>of 3 years for the electricity sector.</t>
   </si>
 </sst>
 </file>
@@ -180,7 +173,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -190,7 +183,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -209,6 +201,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="x_x_Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6796C786-003E-1A25-FAA4-2477005227A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="219075" y="2895600"/>
+          <a:ext cx="9429750" cy="6324600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +588,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,10 +596,10 @@
         <v>0.73</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,77 +612,36 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB35C55-7F27-44A6-A8A7-496D78F28576}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="7">
-        <f>About!B11*About!A9</f>
-        <v>62.05</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="7">
-        <f>B1*B3/B2</f>
-        <v>37.229999999999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -638,7 +649,7 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="F2:G2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,54 +763,57 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="E2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="F2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="G2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="H2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="I2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="J2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="K2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="L2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="M2" s="8">
-        <f>'Electricity Calculations'!$B$4</f>
-        <v>37.229999999999997</v>
+      <c r="D2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="E2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="F2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="G2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="H2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="I2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="J2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="K2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="L2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="M2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -857,7 +871,7 @@
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <f>About!$B$11*About!$A$9</f>
         <v>62.05</v>
       </c>
@@ -957,7 +971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5698252-CD29-4D86-9D7F-2214C5598602}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -972,7 +986,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1">
         <v>2021</v>
@@ -1067,7 +1081,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>12</v>

</xml_diff>

<commit_message>
Remove policies from BAU files
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB3F35D-7F66-4C00-89AD-AA6C0182CF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE7E4E2-0D86-40E4-AC1D-1226986EB12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -183,7 +183,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -553,7 +552,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +606,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -765,55 +764,55 @@
       </c>
       <c r="D2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="L2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="N2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="O2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -871,45 +870,45 @@
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+      <c r="D3">
+        <f>About!$B$11*About!$A$9</f>
+        <v>0</v>
       </c>
       <c r="E3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>0</v>

</xml_diff>

<commit_message>
Update BAU industry CCS subsidies for tax credit duration
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB3F35D-7F66-4C00-89AD-AA6C0182CF63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4853780-9413-4EE5-B529-41F3C3791EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="BCS-BCS" sheetId="4" r:id="rId2"/>
-    <sheet name="BCS-DoSfCS" sheetId="6" r:id="rId3"/>
+    <sheet name="Calculations" sheetId="7" r:id="rId2"/>
+    <sheet name="BCS-BCS" sheetId="4" r:id="rId3"/>
+    <sheet name="BCS-DoSfCS" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">About!$A$11</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Source:</t>
   </si>
@@ -118,6 +119,117 @@
   </si>
   <si>
     <t>of 3 years for the electricity sector.</t>
+  </si>
+  <si>
+    <t>45Q phase-in period</t>
+  </si>
+  <si>
+    <t>45Q phase-out period</t>
+  </si>
+  <si>
+    <t>The potentials below use the "High emissions" values from the Rhodium figure above and are presented as MMT of capture capacity.</t>
+  </si>
+  <si>
+    <t>agriculture and forestry 01T03</t>
+  </si>
+  <si>
+    <t>coal mining 05</t>
+  </si>
+  <si>
+    <t>oil and gas extraction 06</t>
+  </si>
+  <si>
+    <t>other mining and quarrying 07T08</t>
+  </si>
+  <si>
+    <t>food beverage and tobacco 10T12</t>
+  </si>
+  <si>
+    <t>textiles apparel and leather 13T15</t>
+  </si>
+  <si>
+    <t>wood products 16</t>
+  </si>
+  <si>
+    <t>pulp paper and printing 17T18</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19 - energy</t>
+  </si>
+  <si>
+    <t>*mapped to energy-related emissions rather than process emissions, since CCS equipment is installed on crackers</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19 - process</t>
+  </si>
+  <si>
+    <t>*mapped to process emissions</t>
+  </si>
+  <si>
+    <t>chemicals 20</t>
+  </si>
+  <si>
+    <t>*ammonia not counted because we assume this industry is decarbonized through the hydrogen PTC</t>
+  </si>
+  <si>
+    <t>rubber and plastic products 22</t>
+  </si>
+  <si>
+    <t>glass and glass products 231</t>
+  </si>
+  <si>
+    <t>cement and other nonmetallic minerals 239</t>
+  </si>
+  <si>
+    <t>iron and steel 241</t>
+  </si>
+  <si>
+    <t>other metals 242</t>
+  </si>
+  <si>
+    <t>metal products except machinery and vehicles 25</t>
+  </si>
+  <si>
+    <t>computers and electronics 26</t>
+  </si>
+  <si>
+    <t>appliances and electrical equipment 27</t>
+  </si>
+  <si>
+    <t>other machinery 28</t>
+  </si>
+  <si>
+    <t>road vehicles 29</t>
+  </si>
+  <si>
+    <t>nonroad vehicles 30</t>
+  </si>
+  <si>
+    <t>other manufacturing 31T33</t>
+  </si>
+  <si>
+    <t>energy pipelines and gas processing 352T353</t>
+  </si>
+  <si>
+    <t>water and waste 36T39</t>
+  </si>
+  <si>
+    <t>construction 41T43</t>
+  </si>
+  <si>
+    <t>*We use the data below for calculating the fraction of CCS potential achieved by industry. We do not subscript 45Q tax credits by sub-industry, so we must</t>
+  </si>
+  <si>
+    <t>choose a representative value for determining how to apply a duration multiplier. Since most of the incremental CCS comes online between 2030-2035, we use that timeline.</t>
+  </si>
+  <si>
+    <t>The electricity sector calculations properly apply the tax credit duration depending on when CCS capacity comes online.</t>
+  </si>
+  <si>
+    <t>However, the industry sector does not have stock tracking for CCS equipment. Therefore, we adjust the BAU subsidy</t>
+  </si>
+  <si>
+    <t>values for industry only to reflect the duration multiplier.</t>
   </si>
 </sst>
 </file>
@@ -173,7 +285,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -183,6 +295,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -550,25 +665,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="41.81640625" customWidth="1"/>
+    <col min="2" max="2" width="55.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,22 +691,22 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>0.73</v>
       </c>
@@ -602,7 +717,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -610,13 +725,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -624,14 +739,29 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -642,6 +772,551 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1086F14D-0ABA-4CBC-A6C8-8AA6F7BA1ED0}">
+  <dimension ref="A1:AE35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:AE3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B1" s="7">
+        <v>2021</v>
+      </c>
+      <c r="C1">
+        <v>2022</v>
+      </c>
+      <c r="D1" s="7">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2024</v>
+      </c>
+      <c r="F1" s="7">
+        <v>2025</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+      <c r="H1" s="7">
+        <v>2027</v>
+      </c>
+      <c r="I1">
+        <v>2028</v>
+      </c>
+      <c r="J1" s="7">
+        <v>2029</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1" s="7">
+        <v>2031</v>
+      </c>
+      <c r="M1">
+        <v>2032</v>
+      </c>
+      <c r="N1" s="7">
+        <v>2033</v>
+      </c>
+      <c r="O1">
+        <v>2034</v>
+      </c>
+      <c r="P1" s="7">
+        <v>2035</v>
+      </c>
+      <c r="Q1">
+        <v>2036</v>
+      </c>
+      <c r="R1" s="7">
+        <v>2037</v>
+      </c>
+      <c r="S1">
+        <v>2038</v>
+      </c>
+      <c r="T1" s="7">
+        <v>2039</v>
+      </c>
+      <c r="U1">
+        <v>2040</v>
+      </c>
+      <c r="V1" s="7">
+        <v>2041</v>
+      </c>
+      <c r="W1">
+        <v>2042</v>
+      </c>
+      <c r="X1" s="7">
+        <v>2043</v>
+      </c>
+      <c r="Y1">
+        <v>2044</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>2045</v>
+      </c>
+      <c r="AA1">
+        <v>2046</v>
+      </c>
+      <c r="AB1" s="7">
+        <v>2047</v>
+      </c>
+      <c r="AC1">
+        <v>2048</v>
+      </c>
+      <c r="AD1" s="7">
+        <v>2049</v>
+      </c>
+      <c r="AE1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="M2">
+        <f>L2+1/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ref="N2:P2" si="0">M2+1/5</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <f>IFERROR(IF(A3=1,1,INDEX($B$2:$AE$2,MATCH((B1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>IFERROR(IF(B3=1,1,INDEX($B$2:$AE$2,MATCH((C1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>IFERROR(IF(C3=1,1,INDEX($B$2:$AE$2,MATCH((D1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>IFERROR(IF(D3=1,1,INDEX($B$2:$AE$2,MATCH((E1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>IFERROR(IF(E3=1,1,INDEX($B$2:$AE$2,MATCH((F1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>IFERROR(IF(F3=1,1,INDEX($B$2:$AE$2,MATCH((G1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>IFERROR(IF(G3=1,1,INDEX($B$2:$AE$2,MATCH((H1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>IFERROR(IF(H3=1,1,INDEX($B$2:$AE$2,MATCH((I1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>IFERROR(IF(I3=1,1,INDEX($B$2:$AE$2,MATCH((J1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>IFERROR(IF(J3=1,1,INDEX($B$2:$AE$2,MATCH((K1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>IFERROR(IF(K3=1,1,INDEX($B$2:$AE$2,MATCH((L1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>IFERROR(IF(L3=1,1,INDEX($B$2:$AE$2,MATCH((M1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>IFERROR(IF(M3=1,1,INDEX($B$2:$AE$2,MATCH((N1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>IFERROR(IF(N3=1,1,INDEX($B$2:$AE$2,MATCH((O1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>IFERROR(IF(O3=1,1,INDEX($B$2:$AE$2,MATCH((P1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>IFERROR(IF(P3=1,1,INDEX($B$2:$AE$2,MATCH((Q1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>IFERROR(IF(Q3=1,1,INDEX($B$2:$AE$2,MATCH((R1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>IFERROR(IF(R3=1,1,INDEX($B$2:$AE$2,MATCH((S1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>IFERROR(IF(S3=1,1,INDEX($B$2:$AE$2,MATCH((T1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f>IFERROR(IF(T3=1,1,INDEX($B$2:$AE$2,MATCH((U1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f>IFERROR(IF(U3=1,1,INDEX($B$2:$AE$2,MATCH((V1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>IFERROR(IF(V3=1,1,INDEX($B$2:$AE$2,MATCH((W1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f>IFERROR(IF(W3=1,1,INDEX($B$2:$AE$2,MATCH((X1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y3">
+        <f>IFERROR(IF(X3=1,1,INDEX($B$2:$AE$2,MATCH((Y1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0.4</v>
+      </c>
+      <c r="Z3">
+        <f>IFERROR(IF(Y3=1,1,INDEX($B$2:$AE$2,MATCH((Z1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="AA3">
+        <f>IFERROR(IF(Z3=1,1,INDEX($B$2:$AE$2,MATCH((AA1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>0.8</v>
+      </c>
+      <c r="AB3">
+        <f>IFERROR(IF(AA3=1,1,INDEX($B$2:$AE$2,MATCH((AB1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC3">
+        <f>IFERROR(IF(AB3=1,1,INDEX($B$2:$AE$2,MATCH((AC1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <f>IFERROR(IF(AC3=1,1,INDEX($B$2:$AE$2,MATCH((AD1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <f>IFERROR(IF(AD3=1,1,INDEX($B$2:$AE$2,MATCH((AE1-'BCS-DoSfCS'!$B$2),$B$1:$AE$1,0))),0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>2022</v>
+      </c>
+      <c r="C9">
+        <v>2030</v>
+      </c>
+      <c r="D9">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>53</v>
+      </c>
+      <c r="D19">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -649,16 +1324,16 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D2" sqref="D2:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -753,7 +1428,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -763,105 +1438,120 @@
       <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="E2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="F2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="G2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="H2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="I2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="J2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="K2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="L2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="M2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="N2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="O2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="P2">
-        <f>About!$B$11*About!$A$9</f>
-        <v>62.05</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!D3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="E2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!E3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="F2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!F3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="G2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!G3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="H2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!H3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="I2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!I3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="J2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!J3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="K2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!K3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="L2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!L3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="M2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!M3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="N2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!N3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="O2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!O3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="P2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!P3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!Q3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="R2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!R3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="S2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!S3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="T2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!T3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="U2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!U3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="V2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!V3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="W2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!W3)</f>
+        <v>62.05</v>
+      </c>
+      <c r="X2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!X3)</f>
+        <v>49.64</v>
+      </c>
+      <c r="Y2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!Y3)</f>
+        <v>37.229999999999997</v>
+      </c>
+      <c r="Z2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!Z3)</f>
+        <v>24.819999999999993</v>
+      </c>
+      <c r="AA2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AA3)</f>
+        <v>12.409999999999997</v>
+      </c>
+      <c r="AB2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AB3)</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AC3)</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AD3)</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="8">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AE3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -871,7 +1561,7 @@
       <c r="C3" s="4">
         <v>0</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3">
         <f>About!$B$11*About!$A$9</f>
         <v>62.05</v>
       </c>
@@ -971,7 +1661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5698252-CD29-4D86-9D7F-2214C5598602}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -982,9 +1672,9 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -1079,7 +1769,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Correct mismatch in subscript mapping in BCS file
</commit_message>
<xml_diff>
--- a/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
+++ b/InputData/ccs/BCS/BAU CCS Subsidy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4853780-9413-4EE5-B529-41F3C3791EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7519D7CE-E98F-413E-A6DF-5C9601EE62D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -285,20 +285,18 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -667,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +705,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>0.73</v>
       </c>
       <c r="B9" t="s">
@@ -721,7 +719,7 @@
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>85</v>
       </c>
     </row>
@@ -729,7 +727,7 @@
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -785,91 +783,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="B1" s="7">
+      <c r="B1" s="6">
         <v>2021</v>
       </c>
       <c r="C1">
         <v>2022</v>
       </c>
-      <c r="D1" s="7">
+      <c r="D1" s="6">
         <v>2023</v>
       </c>
       <c r="E1">
         <v>2024</v>
       </c>
-      <c r="F1" s="7">
+      <c r="F1" s="6">
         <v>2025</v>
       </c>
       <c r="G1">
         <v>2026</v>
       </c>
-      <c r="H1" s="7">
+      <c r="H1" s="6">
         <v>2027</v>
       </c>
       <c r="I1">
         <v>2028</v>
       </c>
-      <c r="J1" s="7">
+      <c r="J1" s="6">
         <v>2029</v>
       </c>
       <c r="K1">
         <v>2030</v>
       </c>
-      <c r="L1" s="7">
+      <c r="L1" s="6">
         <v>2031</v>
       </c>
       <c r="M1">
         <v>2032</v>
       </c>
-      <c r="N1" s="7">
+      <c r="N1" s="6">
         <v>2033</v>
       </c>
       <c r="O1">
         <v>2034</v>
       </c>
-      <c r="P1" s="7">
+      <c r="P1" s="6">
         <v>2035</v>
       </c>
       <c r="Q1">
         <v>2036</v>
       </c>
-      <c r="R1" s="7">
+      <c r="R1" s="6">
         <v>2037</v>
       </c>
       <c r="S1">
         <v>2038</v>
       </c>
-      <c r="T1" s="7">
+      <c r="T1" s="6">
         <v>2039</v>
       </c>
       <c r="U1">
         <v>2040</v>
       </c>
-      <c r="V1" s="7">
+      <c r="V1" s="6">
         <v>2041</v>
       </c>
       <c r="W1">
         <v>2042</v>
       </c>
-      <c r="X1" s="7">
+      <c r="X1" s="6">
         <v>2043</v>
       </c>
       <c r="Y1">
         <v>2044</v>
       </c>
-      <c r="Z1" s="7">
+      <c r="Z1" s="6">
         <v>2045</v>
       </c>
       <c r="AA1">
         <v>2046</v>
       </c>
-      <c r="AB1" s="7">
+      <c r="AB1" s="6">
         <v>2047</v>
       </c>
       <c r="AC1">
         <v>2048</v>
       </c>
-      <c r="AD1" s="7">
+      <c r="AD1" s="6">
         <v>2049</v>
       </c>
       <c r="AE1">
@@ -1323,8 +1321,8 @@
   </sheetPr>
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:AE2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1432,122 +1430,107 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-      <c r="D2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!D3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="E2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!E3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="F2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!F3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="G2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!G3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="H2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!H3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="I2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!I3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="J2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!J3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="K2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!K3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="L2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!L3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="M2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!M3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="N2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!N3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="O2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!O3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="P2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!P3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="Q2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!Q3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="R2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!R3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="S2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!S3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="T2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!T3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="U2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!U3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="V2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!V3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="W2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!W3)</f>
-        <v>62.05</v>
-      </c>
-      <c r="X2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!X3)</f>
-        <v>49.64</v>
-      </c>
-      <c r="Y2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!Y3)</f>
-        <v>37.229999999999997</v>
-      </c>
-      <c r="Z2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!Z3)</f>
-        <v>24.819999999999993</v>
-      </c>
-      <c r="AA2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!AA3)</f>
-        <v>12.409999999999997</v>
-      </c>
-      <c r="AB2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!AB3)</f>
-        <v>0</v>
-      </c>
-      <c r="AC2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!AC3)</f>
-        <v>0</v>
-      </c>
-      <c r="AD2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!AD3)</f>
-        <v>0</v>
-      </c>
-      <c r="AE2" s="8">
-        <f>About!$B$11*About!$A$9*(1-Calculations!AE3)</f>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="E2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="F2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="G2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="H2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="I2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="J2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="K2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="L2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="M2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="N2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="O2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="P2">
+        <f>About!$B$11*About!$A$9</f>
+        <v>62.05</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
         <v>0</v>
       </c>
     </row>
@@ -1555,104 +1538,122 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!D3)</f>
         <v>62.05</v>
       </c>
       <c r="E3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!E3)</f>
         <v>62.05</v>
       </c>
       <c r="F3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!F3)</f>
         <v>62.05</v>
       </c>
       <c r="G3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!G3)</f>
         <v>62.05</v>
       </c>
       <c r="H3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!H3)</f>
         <v>62.05</v>
       </c>
       <c r="I3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!I3)</f>
         <v>62.05</v>
       </c>
       <c r="J3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!J3)</f>
         <v>62.05</v>
       </c>
       <c r="K3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!K3)</f>
         <v>62.05</v>
       </c>
       <c r="L3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!L3)</f>
         <v>62.05</v>
       </c>
       <c r="M3">
-        <f>About!$B$11*About!$A$9</f>
+        <f>About!$B$11*About!$A$9*(1-Calculations!M3)</f>
         <v>62.05</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!N3)</f>
+        <v>62.05</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!O3)</f>
+        <v>62.05</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!P3)</f>
+        <v>62.05</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!Q3)</f>
+        <v>62.05</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!R3)</f>
+        <v>62.05</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!S3)</f>
+        <v>62.05</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!T3)</f>
+        <v>62.05</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!U3)</f>
+        <v>62.05</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!V3)</f>
+        <v>62.05</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!W3)</f>
+        <v>62.05</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!X3)</f>
+        <v>49.64</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!Y3)</f>
+        <v>37.229999999999997</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!Z3)</f>
+        <v>24.819999999999993</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <f>About!$B$11*About!$A$9*(1-Calculations!AA3)</f>
+        <v>12.409999999999997</v>
       </c>
       <c r="AB3">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AB3)</f>
         <v>0</v>
       </c>
       <c r="AC3">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AC3)</f>
         <v>0</v>
       </c>
       <c r="AD3">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AD3)</f>
         <v>0</v>
       </c>
       <c r="AE3">
+        <f>About!$B$11*About!$A$9*(1-Calculations!AE3)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>